<commit_message>
Resolvendo bug com nomes de equipe diferente nas duas planilhas
</commit_message>
<xml_diff>
--- a/Férias.xlsx
+++ b/Férias.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petrobrasbr-my.sharepoint.com/personal/vinicius_s_duarte_petrobras_com_br/Documents/Área de Trabalho/Teste_Script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{C9AC08D9-4009-4C0A-B1F2-9AC8A478837C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F27C686-80F3-4DBF-A12E-FE59AB9B65AD}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{C9AC08D9-4009-4C0A-B1F2-9AC8A478837C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBFEBB55-22B6-4835-9D7D-C6F063CB1EAC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4FA6F3C-6A0B-4FBC-94DA-2FC748905E27}"/>
   </bookViews>
   <sheets>
     <sheet name="grwRegistros_DVPX_20250915_1257" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">grwRegistros_DVPX_20250915_1257!$A$1:$R$42</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1109,8 +1112,8 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3394,6 +3397,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R42" xr:uid="{F378EF49-324F-4C6D-9B9C-34AB9507E8B5}"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="javascript:__doPostBack('grwRegistros','Sort$Matricula')" xr:uid="{0CCEC443-13CC-49FB-A7F9-55533D6F6E17}"/>
     <hyperlink ref="B1" r:id="rId2" display="javascript:__doPostBack('grwRegistros','Sort$NomeEmpregado')" xr:uid="{DD3708AD-78DA-4F25-9430-DDD7CC4B6002}"/>

</xml_diff>